<commit_message>
update to shapefiles and other scripts
</commit_message>
<xml_diff>
--- a/data-public/raw/old-koatuu-coding.xlsx
+++ b/data-public/raw/old-koatuu-coding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serhii/Desktop/KSE Institute/ua-de-center/data-private/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tytiu\Desktop\KSE\ua-de-center\data-public\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C400194-192D-B240-91BD-6397583C0426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8674CDF-491F-4FB7-B0FC-3B0ACD1FCB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="500" windowWidth="11740" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="497">
   <si>
     <t>area</t>
   </si>
@@ -241,18 +241,6 @@
     <t>Мар’янівка</t>
   </si>
   <si>
-    <t>2321187401</t>
-  </si>
-  <si>
-    <t>Велика Білозерка(Частина 3 Села)</t>
-  </si>
-  <si>
-    <t>2321188401</t>
-  </si>
-  <si>
-    <t>Велика Білозерка(Частина 4 Села)</t>
-  </si>
-  <si>
     <t>4823381301</t>
   </si>
   <si>
@@ -1112,9 +1100,6 @@
   </si>
   <si>
     <t>UA18080090030073587</t>
-  </si>
-  <si>
-    <t>UA23040050010097416</t>
   </si>
   <si>
     <t>UA48060050030044897</t>
@@ -1541,18 +1526,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1567,12 +1546,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1866,21 +1844,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D168"/>
+  <dimension ref="A1:D166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1891,10 +1869,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1905,10 +1883,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1919,10 +1897,10 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1933,10 +1911,10 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1947,10 +1925,10 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1961,10 +1939,10 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1975,10 +1953,10 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1989,10 +1967,10 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2003,10 +1981,10 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2017,10 +1995,10 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2031,10 +2009,10 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -2045,10 +2023,10 @@
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2059,10 +2037,10 @@
         <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2073,10 +2051,10 @@
         <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2087,10 +2065,10 @@
         <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -2101,10 +2079,10 @@
         <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2115,10 +2093,10 @@
         <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2129,10 +2107,10 @@
         <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -2143,10 +2121,10 @@
         <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2157,10 +2135,10 @@
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2171,10 +2149,10 @@
         <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2185,10 +2163,10 @@
         <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2199,10 +2177,10 @@
         <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -2213,10 +2191,10 @@
         <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -2227,10 +2205,10 @@
         <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2241,10 +2219,10 @@
         <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2255,10 +2233,10 @@
         <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -2269,10 +2247,10 @@
         <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -2283,40 +2261,40 @@
         <v>71</v>
       </c>
       <c r="D29" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="D30" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
         <v>78</v>
@@ -2325,236 +2303,236 @@
         <v>77</v>
       </c>
       <c r="D32" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>79</v>
       </c>
-      <c r="D33" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>86</v>
-      </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
         <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>90</v>
       </c>
-      <c r="C37" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>83</v>
-      </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
         <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" t="s">
         <v>93</v>
       </c>
-      <c r="C39" t="s">
-        <v>92</v>
-      </c>
       <c r="D39" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
         <v>95</v>
       </c>
       <c r="D40" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>6</v>
       </c>
       <c r="B41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" t="s">
         <v>98</v>
       </c>
-      <c r="C41" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" t="s">
-        <v>99</v>
-      </c>
-      <c r="D42" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" t="s">
-        <v>101</v>
-      </c>
-      <c r="C43" t="s">
-        <v>100</v>
-      </c>
-      <c r="D43" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>30</v>
-      </c>
-      <c r="B44" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" t="s">
-        <v>102</v>
-      </c>
-      <c r="D44" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D45" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D46" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>55</v>
       </c>
       <c r="B47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" t="s">
         <v>107</v>
       </c>
-      <c r="C47" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" t="s">
-        <v>108</v>
-      </c>
       <c r="D48" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
         <v>110</v>
@@ -2563,12 +2541,12 @@
         <v>109</v>
       </c>
       <c r="D49" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B50" t="s">
         <v>112</v>
@@ -2577,12 +2555,12 @@
         <v>111</v>
       </c>
       <c r="D50" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
         <v>114</v>
@@ -2591,10 +2569,10 @@
         <v>113</v>
       </c>
       <c r="D51" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -2605,12 +2583,12 @@
         <v>115</v>
       </c>
       <c r="D52" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B53" t="s">
         <v>118</v>
@@ -2619,12 +2597,12 @@
         <v>117</v>
       </c>
       <c r="D53" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B54" t="s">
         <v>120</v>
@@ -2633,54 +2611,54 @@
         <v>119</v>
       </c>
       <c r="D54" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
       <c r="C55" t="s">
         <v>121</v>
       </c>
       <c r="D55" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" t="s">
         <v>124</v>
       </c>
-      <c r="C56" t="s">
-        <v>123</v>
-      </c>
-      <c r="D56" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>86</v>
-      </c>
-      <c r="B57" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57" t="s">
-        <v>125</v>
-      </c>
       <c r="D57" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="B58" t="s">
         <v>127</v>
@@ -2689,10 +2667,10 @@
         <v>126</v>
       </c>
       <c r="D58" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -2703,12 +2681,12 @@
         <v>128</v>
       </c>
       <c r="D59" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B60" t="s">
         <v>131</v>
@@ -2717,12 +2695,12 @@
         <v>130</v>
       </c>
       <c r="D60" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
         <v>133</v>
@@ -2731,138 +2709,138 @@
         <v>132</v>
       </c>
       <c r="D61" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" t="s">
+        <v>136</v>
+      </c>
+      <c r="C62" t="s">
+        <v>135</v>
+      </c>
+      <c r="D62" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D63" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64" t="s">
+        <v>140</v>
+      </c>
+      <c r="D64" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>70</v>
-      </c>
-      <c r="B62" t="s">
-        <v>135</v>
-      </c>
-      <c r="C62" t="s">
-        <v>134</v>
-      </c>
-      <c r="D62" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" t="s">
+        <v>142</v>
+      </c>
+      <c r="D65" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>70</v>
-      </c>
-      <c r="B63" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" t="s">
-        <v>136</v>
-      </c>
-      <c r="D63" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" t="s">
+        <v>144</v>
+      </c>
+      <c r="C66" t="s">
+        <v>143</v>
+      </c>
+      <c r="D66" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>138</v>
-      </c>
-      <c r="B64" t="s">
-        <v>140</v>
-      </c>
-      <c r="C64" t="s">
-        <v>139</v>
-      </c>
-      <c r="D64" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" t="s">
+        <v>145</v>
+      </c>
+      <c r="D67" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>83</v>
-      </c>
-      <c r="B65" t="s">
-        <v>142</v>
-      </c>
-      <c r="C65" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>143</v>
-      </c>
-      <c r="B66" t="s">
-        <v>145</v>
-      </c>
-      <c r="C66" t="s">
-        <v>144</v>
-      </c>
-      <c r="D66" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>3</v>
-      </c>
-      <c r="B67" t="s">
-        <v>140</v>
-      </c>
-      <c r="C67" t="s">
-        <v>146</v>
-      </c>
-      <c r="D67" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>148</v>
+        <v>48</v>
       </c>
       <c r="C68" t="s">
         <v>147</v>
       </c>
       <c r="D68" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="B69" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" t="s">
+        <v>151</v>
+      </c>
+      <c r="C70" t="s">
         <v>150</v>
       </c>
-      <c r="C69" t="s">
-        <v>149</v>
-      </c>
-      <c r="D69" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>19</v>
-      </c>
-      <c r="B70" t="s">
-        <v>48</v>
-      </c>
-      <c r="C70" t="s">
-        <v>151</v>
-      </c>
       <c r="D70" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B71" t="s">
         <v>153</v>
@@ -2871,12 +2849,12 @@
         <v>152</v>
       </c>
       <c r="D71" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>46</v>
       </c>
       <c r="B72" t="s">
         <v>155</v>
@@ -2885,12 +2863,12 @@
         <v>154</v>
       </c>
       <c r="D72" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B73" t="s">
         <v>157</v>
@@ -2899,26 +2877,26 @@
         <v>156</v>
       </c>
       <c r="D73" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B74" t="s">
-        <v>159</v>
+        <v>76</v>
       </c>
       <c r="C74" t="s">
         <v>158</v>
       </c>
       <c r="D74" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>49</v>
+        <v>159</v>
       </c>
       <c r="B75" t="s">
         <v>161</v>
@@ -2927,26 +2905,26 @@
         <v>160</v>
       </c>
       <c r="D75" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="C76" t="s">
         <v>162</v>
       </c>
       <c r="D76" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>163</v>
+        <v>19</v>
       </c>
       <c r="B77" t="s">
         <v>165</v>
@@ -2955,12 +2933,12 @@
         <v>164</v>
       </c>
       <c r="D77" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="B78" t="s">
         <v>167</v>
@@ -2969,40 +2947,40 @@
         <v>166</v>
       </c>
       <c r="D78" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>19</v>
+        <v>168</v>
       </c>
       <c r="B79" t="s">
+        <v>170</v>
+      </c>
+      <c r="C79" t="s">
         <v>169</v>
       </c>
-      <c r="C79" t="s">
-        <v>168</v>
-      </c>
       <c r="D79" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>172</v>
+      </c>
+      <c r="C80" t="s">
         <v>171</v>
       </c>
-      <c r="C80" t="s">
-        <v>170</v>
-      </c>
       <c r="D80" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="B81" t="s">
         <v>174</v>
@@ -3011,12 +2989,12 @@
         <v>173</v>
       </c>
       <c r="D81" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82" t="s">
         <v>176</v>
@@ -3025,12 +3003,12 @@
         <v>175</v>
       </c>
       <c r="D82" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B83" t="s">
         <v>178</v>
@@ -3039,12 +3017,12 @@
         <v>177</v>
       </c>
       <c r="D83" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="B84" t="s">
         <v>180</v>
@@ -3053,12 +3031,12 @@
         <v>179</v>
       </c>
       <c r="D84" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B85" t="s">
         <v>182</v>
@@ -3067,12 +3045,12 @@
         <v>181</v>
       </c>
       <c r="D85" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B86" t="s">
         <v>184</v>
@@ -3081,12 +3059,12 @@
         <v>183</v>
       </c>
       <c r="D86" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B87" t="s">
         <v>186</v>
@@ -3095,12 +3073,12 @@
         <v>185</v>
       </c>
       <c r="D87" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B88" t="s">
         <v>188</v>
@@ -3109,12 +3087,12 @@
         <v>187</v>
       </c>
       <c r="D88" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B89" t="s">
         <v>190</v>
@@ -3123,10 +3101,10 @@
         <v>189</v>
       </c>
       <c r="D89" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>41</v>
       </c>
@@ -3137,12 +3115,12 @@
         <v>191</v>
       </c>
       <c r="D90" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
         <v>194</v>
@@ -3151,54 +3129,54 @@
         <v>193</v>
       </c>
       <c r="D91" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>196</v>
+        <v>76</v>
       </c>
       <c r="C92" t="s">
         <v>195</v>
       </c>
       <c r="D92" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="B93" t="s">
+        <v>197</v>
+      </c>
+      <c r="C93" t="s">
+        <v>196</v>
+      </c>
+      <c r="D93" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>30</v>
+      </c>
+      <c r="B94" t="s">
+        <v>199</v>
+      </c>
+      <c r="C94" t="s">
         <v>198</v>
       </c>
-      <c r="C93" t="s">
-        <v>197</v>
-      </c>
-      <c r="D93" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>3</v>
-      </c>
-      <c r="B94" t="s">
-        <v>80</v>
-      </c>
-      <c r="C94" t="s">
-        <v>199</v>
-      </c>
       <c r="D94" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B95" t="s">
         <v>201</v>
@@ -3207,12 +3185,12 @@
         <v>200</v>
       </c>
       <c r="D95" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B96" t="s">
         <v>203</v>
@@ -3221,12 +3199,12 @@
         <v>202</v>
       </c>
       <c r="D96" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B97" t="s">
         <v>205</v>
@@ -3235,12 +3213,12 @@
         <v>204</v>
       </c>
       <c r="D97" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B98" t="s">
         <v>207</v>
@@ -3249,12 +3227,12 @@
         <v>206</v>
       </c>
       <c r="D98" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="B99" t="s">
         <v>209</v>
@@ -3263,12 +3241,12 @@
         <v>208</v>
       </c>
       <c r="D99" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>41</v>
+        <v>139</v>
       </c>
       <c r="B100" t="s">
         <v>211</v>
@@ -3277,12 +3255,12 @@
         <v>210</v>
       </c>
       <c r="D100" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B101" t="s">
         <v>213</v>
@@ -3291,12 +3269,12 @@
         <v>212</v>
       </c>
       <c r="D101" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="B102" t="s">
         <v>215</v>
@@ -3305,12 +3283,12 @@
         <v>214</v>
       </c>
       <c r="D102" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="B103" t="s">
         <v>217</v>
@@ -3319,12 +3297,12 @@
         <v>216</v>
       </c>
       <c r="D103" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="B104" t="s">
         <v>219</v>
@@ -3333,52 +3311,52 @@
         <v>218</v>
       </c>
       <c r="D104" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="B105" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="C105" t="s">
         <v>220</v>
       </c>
       <c r="D105" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="B106" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C106" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D106" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>70</v>
       </c>
       <c r="B107" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="C107" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D107" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>70</v>
       </c>
@@ -3389,12 +3367,12 @@
         <v>225</v>
       </c>
       <c r="D108" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B109" t="s">
         <v>228</v>
@@ -3403,12 +3381,12 @@
         <v>227</v>
       </c>
       <c r="D109" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B110" t="s">
         <v>230</v>
@@ -3417,12 +3395,12 @@
         <v>229</v>
       </c>
       <c r="D110" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>55</v>
+        <v>168</v>
       </c>
       <c r="B111" t="s">
         <v>232</v>
@@ -3431,138 +3409,138 @@
         <v>231</v>
       </c>
       <c r="D111" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>55</v>
       </c>
       <c r="B112" t="s">
-        <v>234</v>
+        <v>29</v>
       </c>
       <c r="C112" t="s">
         <v>233</v>
       </c>
       <c r="D112" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>172</v>
+        <v>79</v>
       </c>
       <c r="B113" t="s">
+        <v>235</v>
+      </c>
+      <c r="C113" t="s">
+        <v>234</v>
+      </c>
+      <c r="D113" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>79</v>
+      </c>
+      <c r="B114" t="s">
+        <v>237</v>
+      </c>
+      <c r="C114" t="s">
         <v>236</v>
       </c>
-      <c r="C113" t="s">
-        <v>235</v>
-      </c>
-      <c r="D113" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>55</v>
-      </c>
-      <c r="B114" t="s">
-        <v>29</v>
-      </c>
-      <c r="C114" t="s">
-        <v>237</v>
-      </c>
       <c r="D114" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>83</v>
+        <v>159</v>
       </c>
       <c r="B115" t="s">
-        <v>239</v>
+        <v>125</v>
       </c>
       <c r="C115" t="s">
         <v>238</v>
       </c>
       <c r="D115" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="B116" t="s">
+        <v>81</v>
+      </c>
+      <c r="C116" t="s">
+        <v>239</v>
+      </c>
+      <c r="D116" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>58</v>
+      </c>
+      <c r="B117" t="s">
         <v>241</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" t="s">
         <v>240</v>
       </c>
-      <c r="D116" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>163</v>
-      </c>
-      <c r="B117" t="s">
-        <v>129</v>
-      </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>242</v>
       </c>
-      <c r="D117" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>6</v>
-      </c>
       <c r="B118" t="s">
-        <v>85</v>
+        <v>244</v>
       </c>
       <c r="C118" t="s">
         <v>243</v>
       </c>
       <c r="D118" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>58</v>
+        <v>245</v>
       </c>
       <c r="B119" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C119" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D119" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>246</v>
+        <v>30</v>
       </c>
       <c r="B120" t="s">
+        <v>249</v>
+      </c>
+      <c r="C120" t="s">
         <v>248</v>
       </c>
-      <c r="C120" t="s">
-        <v>247</v>
-      </c>
       <c r="D120" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>249</v>
+        <v>30</v>
       </c>
       <c r="B121" t="s">
         <v>251</v>
@@ -3571,54 +3549,54 @@
         <v>250</v>
       </c>
       <c r="D121" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="B122" t="s">
-        <v>253</v>
+        <v>74</v>
       </c>
       <c r="C122" t="s">
         <v>252</v>
       </c>
       <c r="D122" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B123" t="s">
+        <v>254</v>
+      </c>
+      <c r="C123" t="s">
+        <v>253</v>
+      </c>
+      <c r="D123" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>67</v>
+      </c>
+      <c r="B124" t="s">
+        <v>256</v>
+      </c>
+      <c r="C124" t="s">
         <v>255</v>
       </c>
-      <c r="C123" t="s">
-        <v>254</v>
-      </c>
-      <c r="D123" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>172</v>
-      </c>
-      <c r="B124" t="s">
-        <v>78</v>
-      </c>
-      <c r="C124" t="s">
-        <v>256</v>
-      </c>
       <c r="D124" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B125" t="s">
         <v>258</v>
@@ -3627,12 +3605,12 @@
         <v>257</v>
       </c>
       <c r="D125" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="B126" t="s">
         <v>260</v>
@@ -3641,12 +3619,12 @@
         <v>259</v>
       </c>
       <c r="D126" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B127" t="s">
         <v>262</v>
@@ -3655,54 +3633,54 @@
         <v>261</v>
       </c>
       <c r="D127" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>138</v>
+        <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="C128" t="s">
         <v>263</v>
       </c>
       <c r="D128" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B129" t="s">
+        <v>265</v>
+      </c>
+      <c r="C129" t="s">
+        <v>264</v>
+      </c>
+      <c r="D129" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>245</v>
+      </c>
+      <c r="B130" t="s">
+        <v>267</v>
+      </c>
+      <c r="C130" t="s">
         <v>266</v>
       </c>
-      <c r="C129" t="s">
-        <v>265</v>
-      </c>
-      <c r="D129" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>19</v>
-      </c>
-      <c r="B130" t="s">
-        <v>253</v>
-      </c>
-      <c r="C130" t="s">
-        <v>267</v>
-      </c>
       <c r="D130" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="B131" t="s">
         <v>269</v>
@@ -3711,82 +3689,82 @@
         <v>268</v>
       </c>
       <c r="D131" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>249</v>
+        <v>30</v>
       </c>
       <c r="B132" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="C132" t="s">
         <v>270</v>
       </c>
       <c r="D132" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>79</v>
+      </c>
+      <c r="B133" t="s">
+        <v>89</v>
+      </c>
+      <c r="C133" t="s">
+        <v>271</v>
+      </c>
+      <c r="D133" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>79</v>
+      </c>
+      <c r="B134" t="s">
+        <v>217</v>
+      </c>
+      <c r="C134" t="s">
+        <v>272</v>
+      </c>
+      <c r="D134" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>30</v>
+      </c>
+      <c r="B135" t="s">
+        <v>274</v>
+      </c>
+      <c r="C135" t="s">
+        <v>273</v>
+      </c>
+      <c r="D135" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>249</v>
-      </c>
-      <c r="B133" t="s">
-        <v>273</v>
-      </c>
-      <c r="C133" t="s">
-        <v>272</v>
-      </c>
-      <c r="D133" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>30</v>
+      </c>
+      <c r="B136" t="s">
+        <v>276</v>
+      </c>
+      <c r="C136" t="s">
+        <v>275</v>
+      </c>
+      <c r="D136" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>30</v>
-      </c>
-      <c r="B134" t="s">
-        <v>236</v>
-      </c>
-      <c r="C134" t="s">
-        <v>274</v>
-      </c>
-      <c r="D134" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>83</v>
-      </c>
-      <c r="B135" t="s">
-        <v>93</v>
-      </c>
-      <c r="C135" t="s">
-        <v>275</v>
-      </c>
-      <c r="D135" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>83</v>
-      </c>
-      <c r="B136" t="s">
-        <v>221</v>
-      </c>
-      <c r="C136" t="s">
-        <v>276</v>
-      </c>
-      <c r="D136" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="B137" t="s">
         <v>278</v>
@@ -3795,110 +3773,110 @@
         <v>277</v>
       </c>
       <c r="D137" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B138" t="s">
-        <v>280</v>
+        <v>217</v>
       </c>
       <c r="C138" t="s">
         <v>279</v>
       </c>
       <c r="D138" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>79</v>
+      </c>
+      <c r="B139" t="s">
+        <v>48</v>
+      </c>
+      <c r="C139" t="s">
+        <v>280</v>
+      </c>
+      <c r="D139" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>282</v>
+      </c>
+      <c r="C140" t="s">
+        <v>281</v>
+      </c>
+      <c r="D140" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>139</v>
+      </c>
+      <c r="B141" t="s">
+        <v>284</v>
+      </c>
+      <c r="C141" t="s">
+        <v>283</v>
+      </c>
+      <c r="D141" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>86</v>
-      </c>
-      <c r="B139" t="s">
-        <v>282</v>
-      </c>
-      <c r="C139" t="s">
-        <v>281</v>
-      </c>
-      <c r="D139" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>55</v>
-      </c>
-      <c r="B140" t="s">
-        <v>221</v>
-      </c>
-      <c r="C140" t="s">
-        <v>283</v>
-      </c>
-      <c r="D140" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>83</v>
-      </c>
-      <c r="B141" t="s">
-        <v>48</v>
-      </c>
-      <c r="C141" t="s">
-        <v>284</v>
-      </c>
-      <c r="D141" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B142" t="s">
-        <v>286</v>
+        <v>129</v>
       </c>
       <c r="C142" t="s">
         <v>285</v>
       </c>
       <c r="D142" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="B143" t="s">
+        <v>287</v>
+      </c>
+      <c r="C143" t="s">
+        <v>286</v>
+      </c>
+      <c r="D143" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>70</v>
+      </c>
+      <c r="B144" t="s">
+        <v>289</v>
+      </c>
+      <c r="C144" t="s">
         <v>288</v>
       </c>
-      <c r="C143" t="s">
-        <v>287</v>
-      </c>
-      <c r="D143" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>143</v>
-      </c>
-      <c r="B144" t="s">
-        <v>133</v>
-      </c>
-      <c r="C144" t="s">
-        <v>289</v>
-      </c>
       <c r="D144" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="B145" t="s">
         <v>291</v>
@@ -3907,12 +3885,12 @@
         <v>290</v>
       </c>
       <c r="D145" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="B146" t="s">
         <v>293</v>
@@ -3921,12 +3899,12 @@
         <v>292</v>
       </c>
       <c r="D146" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B147" t="s">
         <v>295</v>
@@ -3935,12 +3913,12 @@
         <v>294</v>
       </c>
       <c r="D147" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B148" t="s">
         <v>297</v>
@@ -3949,12 +3927,12 @@
         <v>296</v>
       </c>
       <c r="D148" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B149" t="s">
         <v>299</v>
@@ -3963,12 +3941,12 @@
         <v>298</v>
       </c>
       <c r="D149" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B150" t="s">
         <v>301</v>
@@ -3977,10 +3955,10 @@
         <v>300</v>
       </c>
       <c r="D150" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>3</v>
       </c>
@@ -3991,12 +3969,12 @@
         <v>302</v>
       </c>
       <c r="D151" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B152" t="s">
         <v>305</v>
@@ -4005,12 +3983,12 @@
         <v>304</v>
       </c>
       <c r="D152" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B153" t="s">
         <v>307</v>
@@ -4019,54 +3997,54 @@
         <v>306</v>
       </c>
       <c r="D153" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="B154" t="s">
-        <v>309</v>
+        <v>15</v>
       </c>
       <c r="C154" t="s">
         <v>308</v>
       </c>
       <c r="D154" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B155" t="s">
+        <v>310</v>
+      </c>
+      <c r="C155" t="s">
+        <v>309</v>
+      </c>
+      <c r="D155" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>55</v>
+      </c>
+      <c r="B156" t="s">
+        <v>312</v>
+      </c>
+      <c r="C156" t="s">
         <v>311</v>
       </c>
-      <c r="C155" t="s">
-        <v>310</v>
-      </c>
-      <c r="D155" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>13</v>
-      </c>
-      <c r="B156" t="s">
-        <v>15</v>
-      </c>
-      <c r="C156" t="s">
-        <v>312</v>
-      </c>
       <c r="D156" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B157" t="s">
         <v>314</v>
@@ -4075,68 +4053,68 @@
         <v>313</v>
       </c>
       <c r="D157" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="B158" t="s">
-        <v>316</v>
+        <v>176</v>
       </c>
       <c r="C158" t="s">
         <v>315</v>
       </c>
       <c r="D158" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>86</v>
+        <v>6</v>
       </c>
       <c r="B159" t="s">
-        <v>318</v>
+        <v>48</v>
       </c>
       <c r="C159" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D159" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>6</v>
       </c>
       <c r="B160" t="s">
-        <v>180</v>
+        <v>318</v>
       </c>
       <c r="C160" t="s">
+        <v>317</v>
+      </c>
+      <c r="D160" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>52</v>
+      </c>
+      <c r="B161" t="s">
+        <v>320</v>
+      </c>
+      <c r="C161" t="s">
         <v>319</v>
       </c>
-      <c r="D160" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>6</v>
-      </c>
-      <c r="B161" t="s">
-        <v>48</v>
-      </c>
-      <c r="C161" t="s">
-        <v>320</v>
-      </c>
       <c r="D161" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B162" t="s">
         <v>322</v>
@@ -4145,12 +4123,12 @@
         <v>321</v>
       </c>
       <c r="D162" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B163" t="s">
         <v>324</v>
@@ -4159,12 +4137,12 @@
         <v>323</v>
       </c>
       <c r="D163" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="B164" t="s">
         <v>326</v>
@@ -4173,12 +4151,12 @@
         <v>325</v>
       </c>
       <c r="D164" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B165" t="s">
         <v>328</v>
@@ -4187,12 +4165,12 @@
         <v>327</v>
       </c>
       <c r="D165" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B166" t="s">
         <v>330</v>
@@ -4201,35 +4179,7 @@
         <v>329</v>
       </c>
       <c r="D166" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>83</v>
-      </c>
-      <c r="B167" t="s">
-        <v>332</v>
-      </c>
-      <c r="C167" t="s">
-        <v>331</v>
-      </c>
-      <c r="D167" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>58</v>
-      </c>
-      <c r="B168" t="s">
-        <v>334</v>
-      </c>
-      <c r="C168" t="s">
-        <v>333</v>
-      </c>
-      <c r="D168" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>